<commit_message>
Correções reinit, browser privado e espera por elementos interativos
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano\Documents\UiPath\GAVB\Moneytimes\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephano\Documents\UiPath\GAVB\News\Money Times\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522D306D-88E0-4516-AB88-010840A01EBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5123E6B9-9041-4E00-8D2A-48CE13A0C17C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -630,7 +630,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>